<commit_message>
Commit for AICc Era output and codes
</commit_message>
<xml_diff>
--- a/output/ModelOutput.xlsx
+++ b/output/ModelOutput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7188" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7188" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="RawRecruits" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,10 @@
     <sheet name="GAM_FROM PAPER" sheetId="10" r:id="rId10"/>
     <sheet name="GAM_FINAL" sheetId="11" r:id="rId11"/>
     <sheet name="GAMforPaper" sheetId="13" r:id="rId12"/>
+    <sheet name="AICc_Era1_GAM_output" sheetId="14" r:id="rId13"/>
+    <sheet name="AICc_Era1_GAM_forPaper" sheetId="15" r:id="rId14"/>
+    <sheet name="AICc_Era2_GAM_output" sheetId="16" r:id="rId15"/>
+    <sheet name="AICc_Era2_GAM_forPaper" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="426">
   <si>
     <t>Model 1</t>
   </si>
@@ -1232,6 +1236,111 @@
   </si>
   <si>
     <t>Model variables</t>
+  </si>
+  <si>
+    <t>CB females (shortened period)</t>
+  </si>
+  <si>
+    <t>CB females, ovig opilio females</t>
+  </si>
+  <si>
+    <t>CB females, Pacific cod 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM RA</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM (shortened period)</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM, NE wind</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM, SE wind</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM, AO RA</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM, NBT RA</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM, May-July SST</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM (linear), May-July SST</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM, PDO RA</t>
+  </si>
+  <si>
+    <t>CB females + ovig CO females</t>
+  </si>
+  <si>
+    <t>CB females + ovig CO females + FHS TBM</t>
+  </si>
+  <si>
+    <t>CB females + ovig CO females + FHS TBM + Pacific cod RA</t>
+  </si>
+  <si>
+    <t>CB females + ovig CO females + Pacific cod RA</t>
+  </si>
+  <si>
+    <t>CB females + Pacific cod RA</t>
+  </si>
+  <si>
+    <t>CB females + FHS TBM</t>
+  </si>
+  <si>
+    <t>CB females + FHS RA</t>
+  </si>
+  <si>
+    <t>CB females + FHS TBM + NE wind</t>
+  </si>
+  <si>
+    <t>CB females + FHS TBM + SE wind</t>
+  </si>
+  <si>
+    <t>CB females + FHS TBM + AO RA3</t>
+  </si>
+  <si>
+    <t>CB females + FHS TBM + NBT RA3</t>
+  </si>
+  <si>
+    <t>CB females + FHS TBM + SST May-July</t>
+  </si>
+  <si>
+    <t>CB females + FHS TBM (linear) + SST May-July</t>
+  </si>
+  <si>
+    <t>CB females + FHS TBM + PDO RA3</t>
+  </si>
+  <si>
+    <t>CB females + Pacific cod RA3</t>
+  </si>
+  <si>
+    <t>CB females + Pacific cod RA3 + NE wind</t>
+  </si>
+  <si>
+    <t>CB females + Pacific cod RA3 + SE wind</t>
+  </si>
+  <si>
+    <t>CB females + Pacific cod RA3 + AO RA3</t>
+  </si>
+  <si>
+    <t>CB females + Pacific cod RA3 NBT RA3</t>
+  </si>
+  <si>
+    <t>CB females + Pacific cod RA3 + SST May-July</t>
+  </si>
+  <si>
+    <t>CB females + Pacific cod RA3 (linear) + SST May-July</t>
+  </si>
+  <si>
+    <t>CB females + Pacific cod RA3 + PDO RA3</t>
   </si>
 </sst>
 </file>
@@ -2816,7 +2925,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18:F35"/>
+      <selection pane="bottomLeft" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3541,8 +3650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3806,6 +3915,1264 @@
   </sheetData>
   <sortState ref="A2:D18">
     <sortCondition descending="1" ref="C2:C18"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="56" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>371</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10">
+        <v>44.391599999999997</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10">
+        <v>29.846129999999999</v>
+      </c>
+      <c r="C3" s="10">
+        <f>B3-$B$2</f>
+        <v>-14.545469999999998</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>40.326700000000002</v>
+      </c>
+      <c r="C4" s="10">
+        <f t="shared" ref="C4:C15" si="0">B4-$B$2</f>
+        <v>-4.0648999999999944</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10">
+        <v>48.700809999999997</v>
+      </c>
+      <c r="C5" s="10">
+        <f t="shared" si="0"/>
+        <v>4.3092100000000002</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <v>30.695979999999999</v>
+      </c>
+      <c r="C6" s="10">
+        <f t="shared" si="0"/>
+        <v>-13.695619999999998</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10">
+        <v>35.441969999999998</v>
+      </c>
+      <c r="C7" s="10">
+        <f t="shared" si="0"/>
+        <v>-8.9496299999999991</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10">
+        <v>28.84667</v>
+      </c>
+      <c r="C8" s="10">
+        <f t="shared" si="0"/>
+        <v>-15.544929999999997</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10">
+        <v>35.904490000000003</v>
+      </c>
+      <c r="C9" s="10">
+        <f t="shared" si="0"/>
+        <v>-8.4871099999999942</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10">
+        <v>39.576880000000003</v>
+      </c>
+      <c r="C10" s="10">
+        <f t="shared" si="0"/>
+        <v>-4.8147199999999941</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10">
+        <v>37.014949999999999</v>
+      </c>
+      <c r="C11" s="10">
+        <f t="shared" si="0"/>
+        <v>-7.3766499999999979</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10">
+        <v>35.968029999999999</v>
+      </c>
+      <c r="C12" s="10">
+        <f t="shared" si="0"/>
+        <v>-8.423569999999998</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10">
+        <v>36.621989999999997</v>
+      </c>
+      <c r="C13" s="10">
+        <f t="shared" si="0"/>
+        <v>-7.7696100000000001</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10">
+        <v>36.621989999999997</v>
+      </c>
+      <c r="C14" s="10">
+        <f t="shared" si="0"/>
+        <v>-7.7696100000000001</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10">
+        <v>39.710839999999997</v>
+      </c>
+      <c r="C15" s="10">
+        <f t="shared" si="0"/>
+        <v>-4.6807599999999994</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="41"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="41"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="41"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>28.84667</v>
+      </c>
+      <c r="C2">
+        <v>-15.544929999999997</v>
+      </c>
+      <c r="D2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>29.846129999999999</v>
+      </c>
+      <c r="C3">
+        <v>-14.545469999999998</v>
+      </c>
+      <c r="D3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>30.695979999999999</v>
+      </c>
+      <c r="C4">
+        <v>-13.695619999999998</v>
+      </c>
+      <c r="D4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>35.441969999999998</v>
+      </c>
+      <c r="C5">
+        <v>-8.9496299999999991</v>
+      </c>
+      <c r="D5" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>35.904490000000003</v>
+      </c>
+      <c r="C6">
+        <v>-8.4871099999999942</v>
+      </c>
+      <c r="D6" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>35.968029999999999</v>
+      </c>
+      <c r="C7">
+        <v>-8.423569999999998</v>
+      </c>
+      <c r="D7" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>36.621989999999997</v>
+      </c>
+      <c r="C8">
+        <v>-7.7696100000000001</v>
+      </c>
+      <c r="D8" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>36.621989999999997</v>
+      </c>
+      <c r="C9">
+        <v>-7.7696100000000001</v>
+      </c>
+      <c r="D9" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>37.014949999999999</v>
+      </c>
+      <c r="C10">
+        <v>-7.3766499999999979</v>
+      </c>
+      <c r="D10" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>39.576880000000003</v>
+      </c>
+      <c r="C11">
+        <v>-4.8147199999999941</v>
+      </c>
+      <c r="D11" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>39.710839999999997</v>
+      </c>
+      <c r="C12">
+        <v>-4.6807599999999994</v>
+      </c>
+      <c r="D12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>40.326700000000002</v>
+      </c>
+      <c r="C13">
+        <v>-4.0648999999999944</v>
+      </c>
+      <c r="D13" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>44.391599999999997</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>48.700809999999997</v>
+      </c>
+      <c r="C15">
+        <v>4.3092100000000002</v>
+      </c>
+      <c r="D15" t="s">
+        <v>393</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D15">
+    <sortCondition ref="C2:C15"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection sqref="A1:D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>45.301769999999998</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>41.458480000000002</v>
+      </c>
+      <c r="C3">
+        <f>B3-$B$2</f>
+        <v>-3.8432899999999961</v>
+      </c>
+      <c r="D3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>36.760669999999998</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C25" si="0">B4-$B$2</f>
+        <v>-8.5411000000000001</v>
+      </c>
+      <c r="D4" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>37.646970000000003</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>-7.6547999999999945</v>
+      </c>
+      <c r="D5" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>35.225749999999998</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>-10.07602</v>
+      </c>
+      <c r="D6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>33.782389999999999</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>-11.519379999999998</v>
+      </c>
+      <c r="D7" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>44.943750000000001</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>-0.35801999999999623</v>
+      </c>
+      <c r="D8" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>47.688540000000003</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2.3867700000000056</v>
+      </c>
+      <c r="D9" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>44.943750000000001</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>-0.35801999999999623</v>
+      </c>
+      <c r="D10" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>48.093980000000002</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2.7922100000000043</v>
+      </c>
+      <c r="D11" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>50.391179999999999</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>5.0894100000000009</v>
+      </c>
+      <c r="D12" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>29.597300000000001</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>-15.704469999999997</v>
+      </c>
+      <c r="D13" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>36.159930000000003</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>-9.1418399999999949</v>
+      </c>
+      <c r="D14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>43.677590000000002</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>-1.6241799999999955</v>
+      </c>
+      <c r="D15" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>45.916969999999999</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.61520000000000152</v>
+      </c>
+      <c r="D16" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>35.814720000000001</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>-9.4870499999999964</v>
+      </c>
+      <c r="D17" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>33.782389999999999</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>-11.519379999999998</v>
+      </c>
+      <c r="D18" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>37.88617</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>-7.4155999999999977</v>
+      </c>
+      <c r="D19" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>40.173389999999998</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>-5.1283799999999999</v>
+      </c>
+      <c r="D20" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>32.533790000000003</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>-12.767979999999994</v>
+      </c>
+      <c r="D21" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>41.252009999999999</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>-4.0497599999999991</v>
+      </c>
+      <c r="D22" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>38.094299999999997</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>-7.2074700000000007</v>
+      </c>
+      <c r="D23" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>52.453769999999999</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>7.152000000000001</v>
+      </c>
+      <c r="D24" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>32.892420000000001</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>-12.409349999999996</v>
+      </c>
+      <c r="D25" t="s">
+        <v>425</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>29.597300000000001</v>
+      </c>
+      <c r="C2">
+        <v>-15.704469999999997</v>
+      </c>
+      <c r="D2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>32.533790000000003</v>
+      </c>
+      <c r="C3">
+        <v>-12.767979999999994</v>
+      </c>
+      <c r="D3" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>32.892420000000001</v>
+      </c>
+      <c r="C4">
+        <v>-12.409349999999996</v>
+      </c>
+      <c r="D4" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>33.782389999999999</v>
+      </c>
+      <c r="C5">
+        <v>-11.519379999999998</v>
+      </c>
+      <c r="D5" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>33.782389999999999</v>
+      </c>
+      <c r="C6">
+        <v>-11.519379999999998</v>
+      </c>
+      <c r="D6" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>35.225749999999998</v>
+      </c>
+      <c r="C7">
+        <v>-10.07602</v>
+      </c>
+      <c r="D7" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>35.814720000000001</v>
+      </c>
+      <c r="C8">
+        <v>-9.4870499999999964</v>
+      </c>
+      <c r="D8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>36.159930000000003</v>
+      </c>
+      <c r="C9">
+        <v>-9.1418399999999949</v>
+      </c>
+      <c r="D9" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>36.760669999999998</v>
+      </c>
+      <c r="C10">
+        <v>-8.5411000000000001</v>
+      </c>
+      <c r="D10" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>37.646970000000003</v>
+      </c>
+      <c r="C11">
+        <v>-7.6547999999999945</v>
+      </c>
+      <c r="D11" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>37.88617</v>
+      </c>
+      <c r="C12">
+        <v>-7.4155999999999977</v>
+      </c>
+      <c r="D12" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>38.094299999999997</v>
+      </c>
+      <c r="C13">
+        <v>-7.2074700000000007</v>
+      </c>
+      <c r="D13" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>40.173389999999998</v>
+      </c>
+      <c r="C14">
+        <v>-5.1283799999999999</v>
+      </c>
+      <c r="D14" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>41.252009999999999</v>
+      </c>
+      <c r="C15">
+        <v>-4.0497599999999991</v>
+      </c>
+      <c r="D15" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>41.458480000000002</v>
+      </c>
+      <c r="C16">
+        <v>-3.8432899999999961</v>
+      </c>
+      <c r="D16" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>43.677590000000002</v>
+      </c>
+      <c r="C17">
+        <v>-1.6241799999999955</v>
+      </c>
+      <c r="D17" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>44.943750000000001</v>
+      </c>
+      <c r="C18">
+        <v>-0.35801999999999623</v>
+      </c>
+      <c r="D18" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>44.943750000000001</v>
+      </c>
+      <c r="C19">
+        <v>-0.35801999999999623</v>
+      </c>
+      <c r="D19" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>45.301769999999998</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>45.916969999999999</v>
+      </c>
+      <c r="C21">
+        <v>0.61520000000000152</v>
+      </c>
+      <c r="D21" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>47.688540000000003</v>
+      </c>
+      <c r="C22">
+        <v>2.3867700000000056</v>
+      </c>
+      <c r="D22" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>48.093980000000002</v>
+      </c>
+      <c r="C23">
+        <v>2.7922100000000043</v>
+      </c>
+      <c r="D23" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>50.391179999999999</v>
+      </c>
+      <c r="C24">
+        <v>5.0894100000000009</v>
+      </c>
+      <c r="D24" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>52.453769999999999</v>
+      </c>
+      <c r="C25">
+        <v>7.152000000000001</v>
+      </c>
+      <c r="D25" t="s">
+        <v>424</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D25">
+    <sortCondition ref="C2:C25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit for new GAM models
</commit_message>
<xml_diff>
--- a/output/ModelOutput.xlsx
+++ b/output/ModelOutput.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7188" firstSheet="13" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7188" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="RawRecruits" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="431">
   <si>
     <t>Model 1</t>
   </si>
@@ -1277,70 +1277,85 @@
     <t>CB females, flathead sole TBM, PDO RA</t>
   </si>
   <si>
-    <t>CB females + ovig CO females</t>
-  </si>
-  <si>
-    <t>CB females + ovig CO females + FHS TBM</t>
-  </si>
-  <si>
-    <t>CB females + ovig CO females + FHS TBM + Pacific cod RA</t>
-  </si>
-  <si>
-    <t>CB females + ovig CO females + Pacific cod RA</t>
-  </si>
-  <si>
-    <t>CB females + Pacific cod RA</t>
-  </si>
-  <si>
-    <t>CB females + FHS TBM</t>
-  </si>
-  <si>
-    <t>CB females + FHS RA</t>
-  </si>
-  <si>
-    <t>CB females + FHS TBM + NE wind</t>
-  </si>
-  <si>
-    <t>CB females + FHS TBM + SE wind</t>
-  </si>
-  <si>
-    <t>CB females + FHS TBM + AO RA3</t>
-  </si>
-  <si>
-    <t>CB females + FHS TBM + NBT RA3</t>
-  </si>
-  <si>
-    <t>CB females + FHS TBM + SST May-July</t>
-  </si>
-  <si>
-    <t>CB females + FHS TBM (linear) + SST May-July</t>
-  </si>
-  <si>
-    <t>CB females + FHS TBM + PDO RA3</t>
-  </si>
-  <si>
-    <t>CB females + Pacific cod RA3</t>
-  </si>
-  <si>
-    <t>CB females + Pacific cod RA3 + NE wind</t>
-  </si>
-  <si>
-    <t>CB females + Pacific cod RA3 + SE wind</t>
-  </si>
-  <si>
-    <t>CB females + Pacific cod RA3 + AO RA3</t>
-  </si>
-  <si>
-    <t>CB females + Pacific cod RA3 NBT RA3</t>
-  </si>
-  <si>
-    <t>CB females + Pacific cod RA3 + SST May-July</t>
-  </si>
-  <si>
-    <t>CB females + Pacific cod RA3 (linear) + SST May-July</t>
-  </si>
-  <si>
-    <t>CB females + Pacific cod RA3 + PDO RA3</t>
+    <t>CB females, flathead sole TBM 2 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM, NBT 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM, AO 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, flathead sole TBM, PDO 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, ovig CO females</t>
+  </si>
+  <si>
+    <t>CB females, ovig CO females, FHS TBM</t>
+  </si>
+  <si>
+    <t>CB females, ovig CO females, FHS TBM, Pacific cod 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, ovig CO females, Pacific cod 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, Pacific cod  3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, FHS TBM</t>
+  </si>
+  <si>
+    <t>CB females, FHS TBM 2 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, FHS TBM, NE wind</t>
+  </si>
+  <si>
+    <t>CB females, FHS TBM, SE wind</t>
+  </si>
+  <si>
+    <t>CB females, FHS TBM, AO 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, FHS TBM, NBT 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, FHS TBM, SST May-July</t>
+  </si>
+  <si>
+    <t>CB females, FHS TBM (linear), SST May-July</t>
+  </si>
+  <si>
+    <t>CB females, FHS TBM, PDO 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, Pacific cod 3 yr rolling average, NE wind</t>
+  </si>
+  <si>
+    <t>CB females, Pacific cod 3 yr rolling average, SE wind</t>
+  </si>
+  <si>
+    <t>CB females, Pacific cod 3 yr rolling average, AO 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, Pacific cod 3 yr rolling average, NBT 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, Pacific cod 3 yr rolling average, SST May-July</t>
+  </si>
+  <si>
+    <t>CB females, Pacific cod 3 yr rolling average (linear), SST May-July</t>
+  </si>
+  <si>
+    <t>CB females, Pacific cod 3 yr rolling average, PDO 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, AO 3 yr rolling average</t>
+  </si>
+  <si>
+    <t>CB females, , AO 3 yr rolling average</t>
   </si>
 </sst>
 </file>
@@ -3650,8 +3665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3676,114 +3691,114 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="10">
-        <v>83.79</v>
+        <v>55.64</v>
       </c>
       <c r="C2" s="10">
-        <v>2.0600000000000023</v>
+        <v>-26.090000000000003</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B3" s="10">
-        <v>81.73</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>389</v>
+        <v>60.57</v>
+      </c>
+      <c r="C3" s="10">
+        <v>-21.160000000000004</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>338</v>
+        <v>384</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="10">
-        <v>81.37</v>
+        <v>60.93</v>
       </c>
       <c r="C4" s="10">
-        <v>-0.35999999999999943</v>
+        <v>-20.800000000000004</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B5" s="10">
-        <v>79.650000000000006</v>
+        <v>61.29</v>
       </c>
       <c r="C5" s="10">
-        <v>-2.0799999999999983</v>
+        <v>-20.440000000000005</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B6" s="10">
-        <v>67.91</v>
+        <v>61.83</v>
       </c>
       <c r="C6" s="10">
-        <v>-13.820000000000007</v>
+        <v>-19.900000000000006</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B7" s="10">
-        <v>65.5</v>
+        <v>62.92</v>
       </c>
       <c r="C7" s="10">
-        <v>-16.230000000000004</v>
+        <v>-18.810000000000002</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" s="10">
-        <v>65.459999999999994</v>
+        <v>63.38</v>
       </c>
       <c r="C8" s="10">
-        <v>-16.27000000000001</v>
+        <v>-18.350000000000001</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B9" s="10">
-        <v>64.790000000000006</v>
+        <v>63.48</v>
       </c>
       <c r="C9" s="10">
-        <v>-16.939999999999998</v>
+        <v>-18.250000000000007</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3802,119 +3817,119 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B11" s="10">
-        <v>63.48</v>
+        <v>64.790000000000006</v>
       </c>
       <c r="C11" s="10">
-        <v>-18.250000000000007</v>
+        <v>-16.939999999999998</v>
       </c>
       <c r="D11" s="41" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" s="10">
-        <v>63.38</v>
+        <v>65.459999999999994</v>
       </c>
       <c r="C12" s="10">
-        <v>-18.350000000000001</v>
+        <v>-16.27000000000001</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B13" s="10">
-        <v>62.92</v>
+        <v>65.5</v>
       </c>
       <c r="C13" s="10">
-        <v>-18.810000000000002</v>
+        <v>-16.230000000000004</v>
       </c>
       <c r="D13" s="41" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B14" s="10">
-        <v>61.83</v>
+        <v>67.91</v>
       </c>
       <c r="C14" s="10">
-        <v>-19.900000000000006</v>
+        <v>-13.820000000000007</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B15" s="10">
-        <v>61.29</v>
+        <v>79.650000000000006</v>
       </c>
       <c r="C15" s="10">
-        <v>-20.440000000000005</v>
+        <v>-2.0799999999999983</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="10">
-        <v>60.93</v>
+        <v>81.37</v>
       </c>
       <c r="C16" s="10">
-        <v>-20.800000000000004</v>
+        <v>-0.35999999999999943</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B17" s="10">
-        <v>60.57</v>
-      </c>
-      <c r="C17" s="10">
-        <v>-21.160000000000004</v>
+        <v>81.73</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>389</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>384</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="10">
-        <v>55.64</v>
+        <v>83.79</v>
       </c>
       <c r="C18" s="10">
-        <v>-26.090000000000003</v>
+        <v>2.0600000000000023</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:D18">
-    <sortCondition descending="1" ref="C2:C18"/>
+    <sortCondition ref="C2:C18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4185,7 +4200,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4262,7 +4277,7 @@
         <v>-8.9496299999999991</v>
       </c>
       <c r="D5" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -4290,7 +4305,7 @@
         <v>-8.423569999999998</v>
       </c>
       <c r="D7" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -4332,7 +4347,7 @@
         <v>-7.3766499999999979</v>
       </c>
       <c r="D10" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -4360,7 +4375,7 @@
         <v>-4.6807599999999994</v>
       </c>
       <c r="D12" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -4415,16 +4430,16 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection sqref="A1:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -4467,7 +4482,7 @@
         <v>-3.8432899999999961</v>
       </c>
       <c r="D3" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4482,7 +4497,7 @@
         <v>-8.5411000000000001</v>
       </c>
       <c r="D4" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4497,7 +4512,7 @@
         <v>-7.6547999999999945</v>
       </c>
       <c r="D5" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -4512,7 +4527,7 @@
         <v>-10.07602</v>
       </c>
       <c r="D6" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -4527,7 +4542,7 @@
         <v>-11.519379999999998</v>
       </c>
       <c r="D7" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -4542,7 +4557,7 @@
         <v>-0.35801999999999623</v>
       </c>
       <c r="D8" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -4557,7 +4572,7 @@
         <v>2.3867700000000056</v>
       </c>
       <c r="D9" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -4572,7 +4587,7 @@
         <v>-0.35801999999999623</v>
       </c>
       <c r="D10" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -4587,7 +4602,7 @@
         <v>2.7922100000000043</v>
       </c>
       <c r="D11" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -4602,7 +4617,7 @@
         <v>5.0894100000000009</v>
       </c>
       <c r="D12" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -4617,7 +4632,7 @@
         <v>-15.704469999999997</v>
       </c>
       <c r="D13" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -4632,7 +4647,7 @@
         <v>-9.1418399999999949</v>
       </c>
       <c r="D14" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -4647,7 +4662,7 @@
         <v>-1.6241799999999955</v>
       </c>
       <c r="D15" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -4662,7 +4677,7 @@
         <v>0.61520000000000152</v>
       </c>
       <c r="D16" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -4677,7 +4692,7 @@
         <v>-9.4870499999999964</v>
       </c>
       <c r="D17" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -4692,7 +4707,7 @@
         <v>-11.519379999999998</v>
       </c>
       <c r="D18" t="s">
-        <v>418</v>
+        <v>393</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -4707,7 +4722,7 @@
         <v>-7.4155999999999977</v>
       </c>
       <c r="D19" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -4722,7 +4737,7 @@
         <v>-5.1283799999999999</v>
       </c>
       <c r="D20" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -4737,7 +4752,7 @@
         <v>-12.767979999999994</v>
       </c>
       <c r="D21" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -4752,7 +4767,7 @@
         <v>-4.0497599999999991</v>
       </c>
       <c r="D22" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -4767,7 +4782,7 @@
         <v>-7.2074700000000007</v>
       </c>
       <c r="D23" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -4782,7 +4797,7 @@
         <v>7.152000000000001</v>
       </c>
       <c r="D24" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -4797,7 +4812,22 @@
         <v>-12.409349999999996</v>
       </c>
       <c r="D25" t="s">
-        <v>425</v>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>29.892410000000002</v>
+      </c>
+      <c r="C26">
+        <f>B26-B2</f>
+        <v>-15.409359999999996</v>
+      </c>
+      <c r="D26" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -4807,17 +4837,17 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -4845,54 +4875,54 @@
         <v>-15.704469999999997</v>
       </c>
       <c r="D2" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B3">
-        <v>32.533790000000003</v>
+        <v>29.892410000000002</v>
       </c>
       <c r="C3">
-        <v>-12.767979999999994</v>
+        <v>-15.409359999999996</v>
       </c>
       <c r="D3" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>32.892420000000001</v>
+        <v>32.533790000000003</v>
       </c>
       <c r="C4">
-        <v>-12.409349999999996</v>
+        <v>-12.767979999999994</v>
       </c>
       <c r="D4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>33.782389999999999</v>
+        <v>32.892420000000001</v>
       </c>
       <c r="C5">
-        <v>-11.519379999999998</v>
+        <v>-12.409349999999996</v>
       </c>
       <c r="D5" t="s">
-        <v>408</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>33.782389999999999</v>
@@ -4901,180 +4931,180 @@
         <v>-11.519379999999998</v>
       </c>
       <c r="D6" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B7">
-        <v>35.225749999999998</v>
+        <v>33.782389999999999</v>
       </c>
       <c r="C7">
-        <v>-10.07602</v>
+        <v>-11.519379999999998</v>
       </c>
       <c r="D7" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>35.814720000000001</v>
+        <v>35.225749999999998</v>
       </c>
       <c r="C8">
-        <v>-9.4870499999999964</v>
+        <v>-10.07602</v>
       </c>
       <c r="D8" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>36.159930000000003</v>
+        <v>35.814720000000001</v>
       </c>
       <c r="C9">
-        <v>-9.1418399999999949</v>
+        <v>-9.4870499999999964</v>
       </c>
       <c r="D9" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B10">
-        <v>36.760669999999998</v>
+        <v>36.159930000000003</v>
       </c>
       <c r="C10">
-        <v>-8.5411000000000001</v>
+        <v>-9.1418399999999949</v>
       </c>
       <c r="D10" t="s">
-        <v>405</v>
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>37.646970000000003</v>
+        <v>36.760669999999998</v>
       </c>
       <c r="C11">
-        <v>-7.6547999999999945</v>
+        <v>-8.5411000000000001</v>
       </c>
       <c r="D11" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>37.88617</v>
+        <v>37.646970000000003</v>
       </c>
       <c r="C12">
-        <v>-7.4155999999999977</v>
+        <v>-7.6547999999999945</v>
       </c>
       <c r="D12" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B13">
-        <v>38.094299999999997</v>
+        <v>37.88617</v>
       </c>
       <c r="C13">
-        <v>-7.2074700000000007</v>
+        <v>-7.4155999999999977</v>
       </c>
       <c r="D13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B14">
-        <v>40.173389999999998</v>
+        <v>38.094299999999997</v>
       </c>
       <c r="C14">
-        <v>-5.1283799999999999</v>
+        <v>-7.2074700000000007</v>
       </c>
       <c r="D14" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15">
-        <v>41.252009999999999</v>
+        <v>40.173389999999998</v>
       </c>
       <c r="C15">
-        <v>-4.0497599999999991</v>
+        <v>-5.1283799999999999</v>
       </c>
       <c r="D15" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B16">
-        <v>41.458480000000002</v>
+        <v>41.252009999999999</v>
       </c>
       <c r="C16">
-        <v>-3.8432899999999961</v>
+        <v>-4.0497599999999991</v>
       </c>
       <c r="D16" t="s">
-        <v>404</v>
+        <v>425</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B17">
-        <v>43.677590000000002</v>
+        <v>41.458480000000002</v>
       </c>
       <c r="C17">
-        <v>-1.6241799999999955</v>
+        <v>-3.8432899999999961</v>
       </c>
       <c r="D17" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B18">
-        <v>44.943750000000001</v>
+        <v>43.677590000000002</v>
       </c>
       <c r="C18">
-        <v>-0.35801999999999623</v>
+        <v>-1.6241799999999955</v>
       </c>
       <c r="D18" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>44.943750000000001</v>
@@ -5083,96 +5113,110 @@
         <v>-0.35801999999999623</v>
       </c>
       <c r="D19" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>45.301769999999998</v>
+        <v>44.943750000000001</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>-0.35801999999999623</v>
       </c>
       <c r="D20" t="s">
-        <v>338</v>
+        <v>413</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B21">
-        <v>45.916969999999999</v>
+        <v>45.301769999999998</v>
       </c>
       <c r="C21">
-        <v>0.61520000000000152</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>416</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B22">
-        <v>47.688540000000003</v>
+        <v>45.916969999999999</v>
       </c>
       <c r="C22">
-        <v>2.3867700000000056</v>
+        <v>0.61520000000000152</v>
       </c>
       <c r="D22" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>48.093980000000002</v>
+        <v>47.688540000000003</v>
       </c>
       <c r="C23">
-        <v>2.7922100000000043</v>
+        <v>2.3867700000000056</v>
       </c>
       <c r="D23" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24">
-        <v>50.391179999999999</v>
+        <v>48.093980000000002</v>
       </c>
       <c r="C24">
-        <v>5.0894100000000009</v>
+        <v>2.7922100000000043</v>
       </c>
       <c r="D24" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25">
+        <v>50.391179999999999</v>
+      </c>
+      <c r="C25">
+        <v>5.0894100000000009</v>
+      </c>
+      <c r="D25" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>52.453769999999999</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>7.152000000000001</v>
       </c>
-      <c r="D25" t="s">
-        <v>424</v>
+      <c r="D26" t="s">
+        <v>427</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D25">
-    <sortCondition ref="C2:C25"/>
+  <sortState ref="A2:D26">
+    <sortCondition ref="C2:C26"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>